<commit_message>
Improved file path handling and visualisation widgets
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74C7AD6-0306-EB46-8977-1D59EEB704AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E947334F-1C85-D644-850E-3286F2BAF6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="1760" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
@@ -92,12 +92,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={4A039285-96F9-4143-A88F-8C916EDC0AD9}</author>
-    <author>tc={93EFDD1F-5B4C-C447-BA1B-4CBE61F64A50}</author>
+    <author>tc={F6FBAABB-6D44-6E4F-81D0-9394F04F64CC}</author>
     <author>tc={20C96175-6992-8D40-9CA4-4CC3E72DCE98}</author>
-    <author>tc={E3A1BF50-0BC7-1141-AFC5-6E9E0F0C2A71}</author>
     <author>tc={5C0CB34F-CFD5-784B-B25C-DBC14A041E76}</author>
     <author>tc={4E5E7B0D-B6A0-8246-B428-30A869DD781A}</author>
-    <author>tc={18A65550-CF8C-E549-80FA-0DAEB7BD80E9}</author>
+    <author>tc={AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}</author>
     <author>tc={63DBE61C-638E-1240-8046-EAC6C26078CF}</author>
   </authors>
   <commentList>
@@ -109,12 +108,12 @@
     Removed, because no cal scale in file</t>
       </text>
     </comment>
-    <comment ref="C9" authorId="1" shapeId="0" xr:uid="{93EFDD1F-5B4C-C447-BA1B-4CBE61F64A50}">
+    <comment ref="C9" authorId="1" shapeId="0" xr:uid="{F6FBAABB-6D44-6E4F-81D0-9394F04F64CC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Removed because no cal scale in file</t>
+    Removed, because no cal scale in file</t>
       </text>
     </comment>
     <comment ref="B10" authorId="2" shapeId="0" xr:uid="{20C96175-6992-8D40-9CA4-4CC3E72DCE98}">
@@ -125,15 +124,7 @@
     Omitting because scale is not in file</t>
       </text>
     </comment>
-    <comment ref="C10" authorId="3" shapeId="0" xr:uid="{E3A1BF50-0BC7-1141-AFC5-6E9E0F0C2A71}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Omitting for now, because there’s no scale information in the THD files</t>
-      </text>
-    </comment>
-    <comment ref="E11" authorId="4" shapeId="0" xr:uid="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
+    <comment ref="E11" authorId="3" shapeId="0" xr:uid="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -141,7 +132,7 @@
     Need to figure out how to deal with N2O scales</t>
       </text>
     </comment>
-    <comment ref="B12" authorId="5" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
+    <comment ref="B12" authorId="4" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -149,15 +140,15 @@
     Removing this for now, because I can’t handle having the same species on two different Picarros</t>
       </text>
     </comment>
-    <comment ref="C12" authorId="6" shapeId="0" xr:uid="{18A65550-CF8C-E549-80FA-0DAEB7BD80E9}">
+    <comment ref="C12" authorId="5" shapeId="0" xr:uid="{AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Excluded because no scale information in file</t>
+    Removed, because no cal scale in file</t>
       </text>
     </comment>
-    <comment ref="E12" authorId="7" shapeId="0" xr:uid="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
+    <comment ref="E12" authorId="6" shapeId="0" xr:uid="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -170,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="87">
   <si>
     <t>MHD</t>
   </si>
@@ -969,14 +960,11 @@
   <threadedComment ref="B9" dT="2023-08-16T23:43:54.87" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{4A039285-96F9-4143-A88F-8C916EDC0AD9}">
     <text>Removed, because no cal scale in file</text>
   </threadedComment>
-  <threadedComment ref="C9" dT="2023-08-16T23:44:48.21" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{93EFDD1F-5B4C-C447-BA1B-4CBE61F64A50}">
-    <text>Removed because no cal scale in file</text>
+  <threadedComment ref="C9" dT="2023-08-16T23:43:54.87" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{F6FBAABB-6D44-6E4F-81D0-9394F04F64CC}">
+    <text>Removed, because no cal scale in file</text>
   </threadedComment>
   <threadedComment ref="B10" dT="2023-08-16T23:55:29.70" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{20C96175-6992-8D40-9CA4-4CC3E72DCE98}">
     <text>Omitting because scale is not in file</text>
-  </threadedComment>
-  <threadedComment ref="C10" dT="2023-08-03T19:14:34.78" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{E3A1BF50-0BC7-1141-AFC5-6E9E0F0C2A71}">
-    <text>Omitting for now, because there’s no scale information in the THD files</text>
   </threadedComment>
   <threadedComment ref="E11" dT="2023-08-17T10:12:40.61" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
     <text>Need to figure out how to deal with N2O scales</text>
@@ -984,8 +972,8 @@
   <threadedComment ref="B12" dT="2023-07-28T09:57:58.28" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
     <text>Removing this for now, because I can’t handle having the same species on two different Picarros</text>
   </threadedComment>
-  <threadedComment ref="C12" dT="2023-08-16T23:48:01.25" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{18A65550-CF8C-E549-80FA-0DAEB7BD80E9}">
-    <text>Excluded because no scale information in file</text>
+  <threadedComment ref="C12" dT="2023-08-16T23:43:54.87" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}">
+    <text>Removed, because no cal scale in file</text>
   </threadedComment>
   <threadedComment ref="E12" dT="2023-08-17T10:13:28.52" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
     <text>Need to figure out how to convert scales</text>
@@ -3035,7 +3023,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3118,9 +3106,6 @@
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">

</xml_diff>

<commit_message>
Updated GCWerks data through 26th Sept 2023
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E947334F-1C85-D644-850E-3286F2BAF6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F917F5E3-9F99-4E41-99CC-ED4D6B35D439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="1760" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
@@ -94,6 +94,7 @@
     <author>tc={4A039285-96F9-4143-A88F-8C916EDC0AD9}</author>
     <author>tc={F6FBAABB-6D44-6E4F-81D0-9394F04F64CC}</author>
     <author>tc={20C96175-6992-8D40-9CA4-4CC3E72DCE98}</author>
+    <author>tc={FB9995F7-859C-414E-BCF8-DCD3D23B0AF5}</author>
     <author>tc={5C0CB34F-CFD5-784B-B25C-DBC14A041E76}</author>
     <author>tc={4E5E7B0D-B6A0-8246-B428-30A869DD781A}</author>
     <author>tc={AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}</author>
@@ -124,7 +125,15 @@
     Omitting because scale is not in file</t>
       </text>
     </comment>
-    <comment ref="E11" authorId="3" shapeId="0" xr:uid="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
+    <comment ref="C10" authorId="3" shapeId="0" xr:uid="{FB9995F7-859C-414E-BCF8-DCD3D23B0AF5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No scale information in latest files (26th Sept)</t>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="4" shapeId="0" xr:uid="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -132,7 +141,7 @@
     Need to figure out how to deal with N2O scales</t>
       </text>
     </comment>
-    <comment ref="B12" authorId="4" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
+    <comment ref="B12" authorId="5" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -140,7 +149,7 @@
     Removing this for now, because I can’t handle having the same species on two different Picarros</t>
       </text>
     </comment>
-    <comment ref="C12" authorId="5" shapeId="0" xr:uid="{AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}">
+    <comment ref="C12" authorId="6" shapeId="0" xr:uid="{AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -148,7 +157,7 @@
     Removed, because no cal scale in file</t>
       </text>
     </comment>
-    <comment ref="E12" authorId="6" shapeId="0" xr:uid="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
+    <comment ref="E12" authorId="7" shapeId="0" xr:uid="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -161,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="87">
   <si>
     <t>MHD</t>
   </si>
@@ -966,6 +975,9 @@
   <threadedComment ref="B10" dT="2023-08-16T23:55:29.70" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{20C96175-6992-8D40-9CA4-4CC3E72DCE98}">
     <text>Omitting because scale is not in file</text>
   </threadedComment>
+  <threadedComment ref="C10" dT="2023-09-26T15:40:37.04" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{FB9995F7-859C-414E-BCF8-DCD3D23B0AF5}">
+    <text>No scale information in latest files (26th Sept)</text>
+  </threadedComment>
   <threadedComment ref="E11" dT="2023-08-17T10:12:40.61" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
     <text>Need to figure out how to deal with N2O scales</text>
   </threadedComment>
@@ -3023,7 +3035,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3106,6 +3118,9 @@
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">

</xml_diff>

<commit_message>
Release schedule updated now that ZEP and THD Picarro files include calibration scales. Fixes issue #7.
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F917F5E3-9F99-4E41-99CC-ED4D6B35D439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF316A91-2C42-514A-B849-2AFFFC2B9E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="1760" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
@@ -91,17 +91,29 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={4A039285-96F9-4143-A88F-8C916EDC0AD9}</author>
-    <author>tc={F6FBAABB-6D44-6E4F-81D0-9394F04F64CC}</author>
-    <author>tc={20C96175-6992-8D40-9CA4-4CC3E72DCE98}</author>
-    <author>tc={FB9995F7-859C-414E-BCF8-DCD3D23B0AF5}</author>
     <author>tc={5C0CB34F-CFD5-784B-B25C-DBC14A041E76}</author>
     <author>tc={4E5E7B0D-B6A0-8246-B428-30A869DD781A}</author>
     <author>tc={AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}</author>
     <author>tc={63DBE61C-638E-1240-8046-EAC6C26078CF}</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{4A039285-96F9-4143-A88F-8C916EDC0AD9}">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Need to figure out how to deal with N2O scales</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="1" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Removing this for now, because I can’t handle having the same species on two different Picarros</t>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="2" shapeId="0" xr:uid="{AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -109,55 +121,7 @@
     Removed, because no cal scale in file</t>
       </text>
     </comment>
-    <comment ref="C9" authorId="1" shapeId="0" xr:uid="{F6FBAABB-6D44-6E4F-81D0-9394F04F64CC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Removed, because no cal scale in file</t>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="2" shapeId="0" xr:uid="{20C96175-6992-8D40-9CA4-4CC3E72DCE98}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Omitting because scale is not in file</t>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="3" shapeId="0" xr:uid="{FB9995F7-859C-414E-BCF8-DCD3D23B0AF5}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    No scale information in latest files (26th Sept)</t>
-      </text>
-    </comment>
-    <comment ref="E11" authorId="4" shapeId="0" xr:uid="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Need to figure out how to deal with N2O scales</t>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="5" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Removing this for now, because I can’t handle having the same species on two different Picarros</t>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="6" shapeId="0" xr:uid="{AF61A411-FD3F-2440-9A5A-53B8C7C0A5F2}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Removed, because no cal scale in file</t>
-      </text>
-    </comment>
-    <comment ref="E12" authorId="7" shapeId="0" xr:uid="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
+    <comment ref="E12" authorId="3" shapeId="0" xr:uid="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -170,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="87">
   <si>
     <t>MHD</t>
   </si>
@@ -437,7 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -476,12 +440,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -966,18 +924,6 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B9" dT="2023-08-16T23:43:54.87" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{4A039285-96F9-4143-A88F-8C916EDC0AD9}">
-    <text>Removed, because no cal scale in file</text>
-  </threadedComment>
-  <threadedComment ref="C9" dT="2023-08-16T23:43:54.87" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{F6FBAABB-6D44-6E4F-81D0-9394F04F64CC}">
-    <text>Removed, because no cal scale in file</text>
-  </threadedComment>
-  <threadedComment ref="B10" dT="2023-08-16T23:55:29.70" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{20C96175-6992-8D40-9CA4-4CC3E72DCE98}">
-    <text>Omitting because scale is not in file</text>
-  </threadedComment>
-  <threadedComment ref="C10" dT="2023-09-26T15:40:37.04" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{FB9995F7-859C-414E-BCF8-DCD3D23B0AF5}">
-    <text>No scale information in latest files (26th Sept)</text>
-  </threadedComment>
   <threadedComment ref="E11" dT="2023-08-17T10:12:40.61" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
     <text>Need to figure out how to deal with N2O scales</text>
   </threadedComment>
@@ -3035,7 +2981,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3104,22 +3050,10 @@
       <c r="A9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Removed to-do list. Transferred issues to github
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8551D0-D18A-7843-8286-6B381F2D3E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD49101-A661-C54E-BF66-6919F21D8EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="1760" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
@@ -410,7 +410,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -449,12 +449,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2999,7 +2993,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added some tests of the config module
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="ALE"/>
@@ -138,7 +138,7 @@
     <t>hcfc-22</t>
   </si>
   <si>
-    <t>2018-08-31 00:00</t>
+    <t/>
   </si>
   <si>
     <t>hcfc-124</t>
@@ -293,7 +293,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,7 +303,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -316,21 +316,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -431,7 +424,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -446,19 +439,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -478,26 +474,23 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -505,16 +498,16 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -826,72 +819,72 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="3" t="s">
@@ -900,10 +893,10 @@
       <c r="B7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="4" t="s">
@@ -929,51 +922,51 @@
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -992,72 +985,72 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="30" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="3" t="s">
@@ -1066,10 +1059,10 @@
       <c r="B7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="4" t="s">
@@ -1095,71 +1088,71 @@
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1178,72 +1171,72 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="F1" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="3" t="s">
@@ -1255,7 +1248,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="4" t="s">
@@ -1281,25 +1274,25 @@
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="6" t="s">
@@ -1337,37 +1330,37 @@
       <c r="E12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
         <v>84</v>
@@ -1375,19 +1368,19 @@
       <c r="E15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="6" t="s">
@@ -1413,7 +1406,7 @@
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1423,7 +1416,7 @@
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1521,66 +1514,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="29" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="29" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="29" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="29" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="27" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="27" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="27" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="27" width="20.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="3" t="s">
@@ -1589,9 +1582,9 @@
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="6" t="s">
@@ -1610,25 +1603,25 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A9" s="21" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A10" s="24" t="s">
+      <c r="B9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A10" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="25"/>
@@ -1636,8 +1629,8 @@
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A11" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A11" s="18" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="25"/>
@@ -1645,8 +1638,8 @@
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A12" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A12" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="25"/>
@@ -1654,8 +1647,8 @@
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A13" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A13" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="25"/>
@@ -1663,19 +1656,19 @@
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A14" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A14" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="26"/>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="26" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A15" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A15" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="25"/>
@@ -1683,36 +1676,36 @@
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A16" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A16" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="26"/>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A17" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A18" s="24" t="s">
+      <c r="B17" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A18" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B18" s="25"/>
@@ -1720,8 +1713,8 @@
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A19" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A19" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B19" s="25"/>
@@ -1729,8 +1722,8 @@
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A20" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A20" s="18" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="25"/>
@@ -1738,8 +1731,8 @@
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A21" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A21" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B21" s="25"/>
@@ -1747,8 +1740,8 @@
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A22" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A22" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B22" s="25"/>
@@ -1756,8 +1749,8 @@
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A23" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A23" s="18" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="25"/>
@@ -1765,91 +1758,91 @@
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A24" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A24" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="27" t="s">
+      <c r="B24" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A25" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A25" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A26" s="24" t="s">
+      <c r="E25" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A26" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
-      <c r="E26" s="27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A27" s="24" t="s">
+      <c r="E26" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="27" t="s">
+      <c r="B27" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="26"/>
-      <c r="E27" s="27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A28" s="24" t="s">
+      <c r="E27" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A29" s="24" t="s">
+      <c r="B28" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A29" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="27" t="s">
+      <c r="B29" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="26"/>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1865,333 +1858,333 @@
   </sheetPr>
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="19.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="8" t="s">
+      <c r="B4" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="8" t="s">
+      <c r="B5" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="11" t="s">
+      <c r="B6" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="12" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A9" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A10" s="15" t="s">
+      <c r="B9" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A11" s="15" t="s">
+      <c r="B10" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A12" s="15" t="s">
+      <c r="B11" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A13" s="15" t="s">
+      <c r="B12" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A14" s="15" t="s">
+      <c r="B13" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A15" s="15" t="s">
+      <c r="B14" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="15">
+      <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A16" s="15" t="s">
+      <c r="B15" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A17" s="15" t="s">
+      <c r="B16" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A18" s="15" t="s">
+      <c r="B17" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A18" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A19" s="15" t="s">
+      <c r="B18" s="17"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A20" s="15" t="s">
+      <c r="B19" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A20" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A21" s="15" t="s">
+      <c r="B20" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A21" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A22" s="15" t="s">
+      <c r="B21" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A22" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A23" s="15" t="s">
+      <c r="B22" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A23" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A24" s="15" t="s">
+      <c r="B23" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A24" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A25" s="15" t="s">
+      <c r="B24" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A25" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A26" s="15" t="s">
+      <c r="B25" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A26" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A27" s="15" t="s">
+      <c r="B26" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A28" s="15" t="s">
+      <c r="B27" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A28" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A29" s="15" t="s">
+      <c r="B28" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A30" s="15" t="s">
+      <c r="B29" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A30" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A31" s="15" t="s">
+      <c r="B30" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A31" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A32" s="15" t="s">
+      <c r="B31" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A32" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A33" s="15" t="s">
+      <c r="B32" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A33" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A34" s="15" t="s">
+      <c r="B33" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A34" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A35" s="15" t="s">
+      <c r="B34" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A35" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A36" s="15" t="s">
+      <c r="B35" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A36" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A37" s="15" t="s">
+      <c r="B36" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A37" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A38" s="15" t="s">
+      <c r="B37" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A38" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A39" s="15" t="s">
+      <c r="B38" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A39" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A40" s="15" t="s">
+      <c r="B39" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A40" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A41" s="15" t="s">
+      <c r="B40" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A41" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A42" s="15" t="s">
+      <c r="B41" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A42" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A43" s="15" t="s">
+      <c r="B42" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A43" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A44" s="15" t="s">
+      <c r="B43" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A44" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A45" s="15" t="s">
+      <c r="B44" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A45" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A46" s="15" t="s">
+      <c r="B45" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A46" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A47" s="15" t="s">
+      <c r="B46" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A48" s="15" t="s">
+      <c r="B47" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A48" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A49" s="15" t="s">
+      <c r="B48" s="18"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A49" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="17"/>
+      <c r="B49" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2205,881 +2198,881 @@
   </sheetPr>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="19" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="19" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="19" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="19" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="19" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="19" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="19" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="20" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="20" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="20" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="20" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="20" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="20" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="20" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="20" width="19.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A9" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="17" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A10" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A11" s="15" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A12" s="15" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="17" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A13" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A14" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A15" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A16" s="15" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A17" s="15" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A18" s="15" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A18" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A19" s="15" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A20" s="15" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A20" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A21" s="15" t="s">
+      <c r="I20" s="18"/>
+      <c r="J20" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A21" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A22" s="15" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A22" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A23" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A23" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A24" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A24" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A25" s="15" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A25" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A26" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A26" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17" t="s">
+      <c r="B26" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A27" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17" t="s">
+      <c r="B27" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A28" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A28" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="17" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A29" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="17" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A30" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A30" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A31" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A31" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17" t="s">
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A32" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A32" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17" t="s">
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A33" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A33" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17" t="s">
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A34" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A34" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="17" t="s">
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A35" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A35" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A36" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A36" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A37" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A37" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A38" s="15" t="s">
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A38" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17" t="s">
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A39" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A39" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17" t="s">
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A40" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A40" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17" t="s">
+      <c r="B40" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A41" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A41" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A42" s="15" t="s">
+      <c r="C41" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A42" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A43" s="15" t="s">
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A43" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J43" s="17" t="s">
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A44" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A44" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A45" s="15" t="s">
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A45" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A46" s="15" t="s">
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A46" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" s="17" t="s">
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A47" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J47" s="17" t="s">
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A48" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A48" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17" t="s">
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" customFormat="1" s="14">
-      <c r="A49" s="15" t="s">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" customFormat="1" s="15">
+      <c r="A49" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="17" t="s">
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3100,44 +3093,44 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="3" t="s">
@@ -3159,7 +3152,7 @@
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated TAC release schedule and added an error if a site/species is missing from release schedule
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683DA10F-DCD3-444F-9026-B388CEBA7105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA78B842-445C-BA47-9AFD-DD4BD054F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="500" windowWidth="26100" windowHeight="19140" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10360" yWindow="500" windowWidth="26100" windowHeight="19140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALE" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="90">
   <si>
     <t># AGAGE GCMD data release schedule</t>
   </si>
@@ -305,7 +305,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +350,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -438,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -532,6 +538,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -944,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD14C28-F730-FB41-A4AA-30BAAD642BC7}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1139,9 +1154,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1152,37 +1169,37 @@
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1190,7 +1207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1209,24 +1226,33 @@
       <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G8" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>75</v>
       </c>
@@ -1245,8 +1271,11 @@
       <c r="F11" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G11" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>61</v>
       </c>
@@ -1262,16 +1291,22 @@
       <c r="E12" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G13" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -1279,7 +1314,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1289,16 +1324,22 @@
       <c r="E15" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -1318,7 +1359,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
@@ -1329,6 +1370,9 @@
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2102,9 +2146,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2113,7 +2159,7 @@
     <col min="3" max="10" width="19" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2127,7 +2173,7 @@
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2141,7 +2187,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -2155,7 +2201,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2169,7 +2215,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -2183,7 +2229,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -2197,7 +2243,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2213,7 +2259,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -2244,8 +2290,11 @@
       <c r="J8" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K8" s="33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -2263,7 +2312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>27</v>
       </c>
@@ -2279,7 +2328,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>28</v>
       </c>
@@ -2295,7 +2344,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>29</v>
       </c>
@@ -2311,7 +2360,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>30</v>
       </c>
@@ -2327,7 +2376,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>31</v>
       </c>
@@ -2343,7 +2392,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>32</v>
       </c>
@@ -2359,7 +2408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>33</v>
       </c>
@@ -2661,7 +2710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>52</v>
       </c>
@@ -2677,7 +2726,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>54</v>
       </c>
@@ -2695,7 +2744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>55</v>
       </c>
@@ -2711,7 +2760,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
         <v>56</v>
       </c>
@@ -2727,7 +2776,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
         <v>57</v>
       </c>
@@ -2745,7 +2794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>59</v>
       </c>
@@ -2763,7 +2812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>61</v>
       </c>
@@ -2779,7 +2828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>62</v>
       </c>
@@ -2807,7 +2856,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>63</v>
       </c>
@@ -2838,8 +2887,11 @@
       <c r="J41" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K41" s="34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>65</v>
       </c>
@@ -2855,7 +2907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>66</v>
       </c>
@@ -2873,7 +2925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>67</v>
       </c>
@@ -2889,7 +2941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
         <v>68</v>
       </c>
@@ -2907,7 +2959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>69</v>
       </c>
@@ -2925,7 +2977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>70</v>
       </c>
@@ -2943,7 +2995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>71</v>
       </c>
@@ -3056,48 +3108,51 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3105,7 +3160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3121,8 +3176,11 @@
       <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F8" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -3130,12 +3188,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -3151,8 +3209,11 @@
       <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -3165,8 +3226,11 @@
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
@@ -3180,6 +3244,9 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add TOB to data_release_schedule.xlsx GCMS-Medusa
exclude TOB data for hcfc-132b, toluene, benzene. I feel this is redundand information on what I already gave in data_combination.xlsx
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Python_Projects\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA78B842-445C-BA47-9AFD-DD4BD054F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="500" windowWidth="26100" windowHeight="19140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10365" yWindow="495" windowWidth="26100" windowHeight="19140" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ALE" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="93">
   <si>
     <t># AGAGE GCMD data release schedule</t>
   </si>
@@ -299,12 +298,21 @@
   </si>
   <si>
     <t># AGAGE LGR data release schedule</t>
+  </si>
+  <si>
+    <t>TOB</t>
+  </si>
+  <si>
+    <t>toluene</t>
+  </si>
+  <si>
+    <t>benzene</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -543,16 +551,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{D7750139-83C2-534B-B787-8EF88849869C}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -851,7 +863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -859,45 +871,45 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -905,7 +917,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -925,27 +937,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -956,50 +968,50 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD14C28-F730-FB41-A4AA-30BAAD642BC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.83203125" style="27"/>
+    <col min="2" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>6</v>
       </c>
@@ -1007,7 +1019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>8</v>
       </c>
@@ -1015,13 +1027,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="28"/>
     </row>
-    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>17</v>
       </c>
@@ -1033,7 +1045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1041,46 +1053,46 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1100,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1108,37 +1120,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1150,56 +1162,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1207,7 +1219,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1226,11 +1238,11 @@
       <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
@@ -1241,7 +1253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
@@ -1252,7 +1264,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>75</v>
       </c>
@@ -1275,7 +1287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>61</v>
       </c>
@@ -1295,7 +1307,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>62</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -1314,7 +1326,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1328,7 +1340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>59</v>
       </c>
@@ -1339,7 +1351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -1359,7 +1371,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
@@ -1382,7 +1394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1390,43 +1402,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1434,7 +1446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1442,7 +1454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
@@ -1456,7 +1468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1464,14 +1476,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.5" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1492,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1489,7 +1501,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1498,7 +1510,7 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1507,7 +1519,7 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1516,7 +1528,7 @@
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1525,7 +1537,7 @@
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1536,7 +1548,7 @@
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1553,7 +1565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>25</v>
       </c>
@@ -1570,7 +1582,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>28</v>
       </c>
@@ -1579,7 +1591,7 @@
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
@@ -1588,7 +1600,7 @@
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>31</v>
       </c>
@@ -1597,7 +1609,7 @@
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
     </row>
-    <row r="13" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>35</v>
       </c>
@@ -1606,7 +1618,7 @@
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>37</v>
       </c>
@@ -1617,7 +1629,7 @@
       </c>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>43</v>
       </c>
@@ -1626,7 +1638,7 @@
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>44</v>
       </c>
@@ -1637,7 +1649,7 @@
       </c>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>48</v>
       </c>
@@ -1654,7 +1666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>51</v>
       </c>
@@ -1663,7 +1675,7 @@
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>52</v>
       </c>
@@ -1672,7 +1684,7 @@
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>55</v>
       </c>
@@ -1681,7 +1693,7 @@
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
     </row>
-    <row r="21" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>56</v>
       </c>
@@ -1690,7 +1702,7 @@
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>57</v>
       </c>
@@ -1699,7 +1711,7 @@
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
     </row>
-    <row r="23" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>59</v>
       </c>
@@ -1708,7 +1720,7 @@
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
     </row>
-    <row r="24" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>61</v>
       </c>
@@ -1721,7 +1733,7 @@
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
     </row>
-    <row r="25" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>63</v>
       </c>
@@ -1738,7 +1750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>65</v>
       </c>
@@ -1749,7 +1761,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>32</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>33</v>
       </c>
@@ -1781,7 +1793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>34</v>
       </c>
@@ -1802,7 +1814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1810,49 +1822,49 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
     </row>
-    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="8"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +1872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -1868,7 +1880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -1876,61 +1888,61 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="14"/>
     </row>
-    <row r="11" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="14"/>
     </row>
-    <row r="12" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="14"/>
     </row>
-    <row r="13" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="14"/>
     </row>
-    <row r="14" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="14"/>
     </row>
-    <row r="15" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="14"/>
     </row>
-    <row r="16" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="14"/>
     </row>
-    <row r="17" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="14"/>
     </row>
-    <row r="18" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="14"/>
     </row>
-    <row r="19" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>36</v>
       </c>
@@ -1938,13 +1950,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>39</v>
       </c>
@@ -1952,43 +1964,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="15"/>
     </row>
-    <row r="23" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="15"/>
     </row>
-    <row r="27" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="15"/>
     </row>
-    <row r="28" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>47</v>
       </c>
@@ -1996,7 +2008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>48</v>
       </c>
@@ -2004,31 +2016,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="15"/>
     </row>
-    <row r="31" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="15"/>
     </row>
-    <row r="32" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="15"/>
     </row>
-    <row r="33" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B33" s="15"/>
     </row>
-    <row r="34" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>54</v>
       </c>
@@ -2036,43 +2048,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>55</v>
       </c>
       <c r="B35" s="15"/>
     </row>
-    <row r="36" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>56</v>
       </c>
       <c r="B36" s="15"/>
     </row>
-    <row r="37" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B37" s="15"/>
     </row>
-    <row r="38" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B38" s="15"/>
     </row>
-    <row r="39" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>61</v>
       </c>
       <c r="B39" s="15"/>
     </row>
-    <row r="40" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>62</v>
       </c>
       <c r="B40" s="15"/>
     </row>
-    <row r="41" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>63</v>
       </c>
@@ -2080,13 +2092,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>65</v>
       </c>
       <c r="B42" s="15"/>
     </row>
-    <row r="43" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>66</v>
       </c>
@@ -2094,13 +2106,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>67</v>
       </c>
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>68</v>
       </c>
@@ -2108,7 +2120,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>69</v>
       </c>
@@ -2116,7 +2128,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>70</v>
       </c>
@@ -2124,13 +2136,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>71</v>
       </c>
       <c r="B48" s="15"/>
     </row>
-    <row r="49" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>72</v>
       </c>
@@ -2142,24 +2154,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="19" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2173,7 +2185,7 @@
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2187,7 +2199,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -2201,7 +2213,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2215,7 +2227,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -2229,7 +2241,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -2243,7 +2255,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2259,7 +2271,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -2293,8 +2305,11 @@
       <c r="K8" s="33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L8" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -2311,8 +2326,10 @@
       <c r="J9" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+    </row>
+    <row r="10" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>27</v>
       </c>
@@ -2327,8 +2344,10 @@
       <c r="J10" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+    </row>
+    <row r="11" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>28</v>
       </c>
@@ -2343,8 +2362,10 @@
       <c r="J11" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+    </row>
+    <row r="12" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>29</v>
       </c>
@@ -2359,8 +2380,10 @@
       <c r="J12" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>30</v>
       </c>
@@ -2375,8 +2398,10 @@
       <c r="J13" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+    </row>
+    <row r="14" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>31</v>
       </c>
@@ -2391,8 +2416,10 @@
       <c r="J14" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+    </row>
+    <row r="15" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>32</v>
       </c>
@@ -2407,8 +2434,10 @@
       <c r="J15" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+    </row>
+    <row r="16" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>33</v>
       </c>
@@ -2423,8 +2452,10 @@
       <c r="J16" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+    </row>
+    <row r="17" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>34</v>
       </c>
@@ -2439,8 +2470,10 @@
       <c r="J17" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+    </row>
+    <row r="18" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>35</v>
       </c>
@@ -2455,8 +2488,10 @@
       <c r="J18" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>36</v>
       </c>
@@ -2473,8 +2508,10 @@
       <c r="J19" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+    </row>
+    <row r="20" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>37</v>
       </c>
@@ -2491,8 +2528,10 @@
       <c r="J20" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+    </row>
+    <row r="21" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>39</v>
       </c>
@@ -2509,8 +2548,10 @@
       <c r="J21" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+    </row>
+    <row r="22" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>40</v>
       </c>
@@ -2525,8 +2566,12 @@
       <c r="J22" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K22" s="35"/>
+      <c r="L22" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>42</v>
       </c>
@@ -2541,8 +2586,10 @@
       <c r="J23" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+    </row>
+    <row r="24" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>43</v>
       </c>
@@ -2557,8 +2604,10 @@
       <c r="J24" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+    </row>
+    <row r="25" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>44</v>
       </c>
@@ -2573,8 +2622,10 @@
       <c r="J25" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+    </row>
+    <row r="26" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>45</v>
       </c>
@@ -2599,8 +2650,10 @@
       <c r="J26" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>46</v>
       </c>
@@ -2625,8 +2678,10 @@
       <c r="J27" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+    </row>
+    <row r="28" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>47</v>
       </c>
@@ -2643,8 +2698,10 @@
       <c r="J28" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+    </row>
+    <row r="29" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>48</v>
       </c>
@@ -2661,8 +2718,10 @@
       <c r="J29" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+    </row>
+    <row r="30" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>49</v>
       </c>
@@ -2677,8 +2736,10 @@
       <c r="J30" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+    </row>
+    <row r="31" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>50</v>
       </c>
@@ -2693,8 +2754,10 @@
       <c r="J31" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+    </row>
+    <row r="32" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>51</v>
       </c>
@@ -2709,8 +2772,10 @@
       <c r="J32" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+    </row>
+    <row r="33" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>52</v>
       </c>
@@ -2725,8 +2790,10 @@
       <c r="J33" s="15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+    </row>
+    <row r="34" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>54</v>
       </c>
@@ -2743,8 +2810,10 @@
       <c r="J34" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+    </row>
+    <row r="35" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>55</v>
       </c>
@@ -2759,8 +2828,10 @@
       <c r="J35" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+    </row>
+    <row r="36" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>56</v>
       </c>
@@ -2775,8 +2846,10 @@
       <c r="J36" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+    </row>
+    <row r="37" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>57</v>
       </c>
@@ -2793,8 +2866,10 @@
       <c r="J37" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+    </row>
+    <row r="38" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>59</v>
       </c>
@@ -2811,8 +2886,10 @@
       <c r="J38" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+    </row>
+    <row r="39" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>61</v>
       </c>
@@ -2827,8 +2904,10 @@
       <c r="J39" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+    </row>
+    <row r="40" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>62</v>
       </c>
@@ -2855,8 +2934,10 @@
       <c r="J40" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+    </row>
+    <row r="41" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>63</v>
       </c>
@@ -2887,11 +2968,12 @@
       <c r="J41" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K41" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K41" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L41" s="35"/>
+    </row>
+    <row r="42" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>65</v>
       </c>
@@ -2906,8 +2988,10 @@
       <c r="J42" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+    </row>
+    <row r="43" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>66</v>
       </c>
@@ -2924,8 +3008,10 @@
       <c r="J43" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+    </row>
+    <row r="44" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>67</v>
       </c>
@@ -2940,8 +3026,10 @@
       <c r="J44" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+    </row>
+    <row r="45" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>68</v>
       </c>
@@ -2958,8 +3046,10 @@
       <c r="J45" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+    </row>
+    <row r="46" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>69</v>
       </c>
@@ -2976,8 +3066,10 @@
       <c r="J46" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+    </row>
+    <row r="47" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>70</v>
       </c>
@@ -2994,8 +3086,10 @@
       <c r="J47" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K47" s="35"/>
+      <c r="L47" s="35"/>
+    </row>
+    <row r="48" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>71</v>
       </c>
@@ -3010,8 +3104,10 @@
       <c r="J48" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
+    </row>
+    <row r="49" spans="1:12" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>72</v>
       </c>
@@ -3026,6 +3122,38 @@
       <c r="J49" s="15" t="s">
         <v>26</v>
       </c>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3033,7 +3161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3041,43 +3169,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3085,7 +3213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3093,7 +3221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -3104,7 +3232,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3114,45 +3242,45 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3160,7 +3288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3180,7 +3308,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -3188,12 +3316,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -3213,7 +3341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -3230,7 +3358,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Remove spurious species from TOB ToF release schedule
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/dagage2_home/code/agage-archive/data/agage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp47837\user\home\zh21490\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059386E6-C138-FF49-A9A5-179371918845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA739285-F331-4B4A-BC2E-AB213CD77ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="29100" windowHeight="15620" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALE" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="98">
   <si>
     <t># AGAGE LGR data release schedule</t>
   </si>
@@ -137,15 +137,6 @@
     <t>hfc-365mfc</t>
   </si>
   <si>
-    <t>hfo-1234yf</t>
-  </si>
-  <si>
-    <t>hfo-1234zee</t>
-  </si>
-  <si>
-    <t>hcfo-1233zde</t>
-  </si>
-  <si>
     <t>hcfc-22</t>
   </si>
   <si>
@@ -170,46 +161,22 @@
     <t>ch3br</t>
   </si>
   <si>
-    <t>ch3i</t>
-  </si>
-  <si>
     <t>ch2cl2</t>
   </si>
   <si>
     <t>chcl3</t>
   </si>
   <si>
-    <t>ch2br2</t>
-  </si>
-  <si>
-    <t>chbr3</t>
-  </si>
-  <si>
     <t>chclccl2</t>
   </si>
   <si>
     <t>ccl2ccl2</t>
   </si>
   <si>
-    <t>clch2ch2cl</t>
-  </si>
-  <si>
-    <t>c2h2</t>
-  </si>
-  <si>
-    <t>c3h8</t>
-  </si>
-  <si>
-    <t>c3h6</t>
-  </si>
-  <si>
     <t>c6h6</t>
   </si>
   <si>
     <t>c6h5ch3</t>
-  </si>
-  <si>
-    <t>cos</t>
   </si>
   <si>
     <t>CMN</t>
@@ -905,94 +872,94 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -1013,14 +980,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1028,7 +995,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1036,7 +1003,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1044,7 +1011,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1052,7 +1019,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1027,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1068,17 +1035,17 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1092,7 +1059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1069,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1110,7 +1077,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1124,7 +1091,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1136,7 +1103,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1166,58 +1133,58 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1228,19 +1195,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1264,58 +1231,58 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1326,7 +1293,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1335,7 +1302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1344,7 +1311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1352,7 +1319,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1360,7 +1327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1387,57 +1354,57 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1445,7 +1412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -1473,61 +1440,61 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1535,13 +1502,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -1563,116 +1530,116 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="40"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="40"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="40"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="40"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="40"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="40"/>
     </row>
-    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B9" s="40"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B10" s="40"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B11" s="40"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B12" s="40"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B13" s="40"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="40"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1697,17 +1664,17 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1716,7 +1683,7 @@
       <c r="E1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1725,7 +1692,7 @@
       <c r="E2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1734,7 +1701,7 @@
       <c r="E3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1743,7 +1710,7 @@
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1752,7 +1719,7 @@
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1761,24 +1728,24 @@
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>18</v>
@@ -1787,7 +1754,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>12</v>
@@ -1796,139 +1763,139 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
         <v>94</v>
       </c>
-      <c r="F15" t="s">
-        <v>105</v>
-      </c>
       <c r="G15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
@@ -1949,7 +1916,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
@@ -1982,59 +1949,59 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -2045,12 +2012,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2069,16 +2036,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2087,7 +2054,7 @@
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2096,7 +2063,7 @@
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2105,7 +2072,7 @@
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2114,7 +2081,7 @@
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2123,7 +2090,7 @@
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2132,35 +2099,35 @@
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
@@ -2169,7 +2136,7 @@
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
     </row>
-    <row r="10" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>28</v>
       </c>
@@ -2178,7 +2145,7 @@
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
     </row>
-    <row r="11" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>30</v>
       </c>
@@ -2187,7 +2154,7 @@
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
     </row>
-    <row r="12" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>33</v>
       </c>
@@ -2196,9 +2163,9 @@
       <c r="D12" s="35"/>
       <c r="E12" s="35"/>
     </row>
-    <row r="13" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
@@ -2207,18 +2174,18 @@
       </c>
       <c r="E13" s="35"/>
     </row>
-    <row r="14" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="35"/>
       <c r="D14" s="35"/>
       <c r="E14" s="35"/>
     </row>
-    <row r="15" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="35"/>
@@ -2227,78 +2194,78 @@
       </c>
       <c r="E15" s="35"/>
     </row>
-    <row r="16" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="36" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="34"/>
       <c r="C17" s="35"/>
       <c r="D17" s="35"/>
       <c r="E17" s="35"/>
     </row>
-    <row r="18" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B18" s="34"/>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
     </row>
-    <row r="19" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="35"/>
       <c r="D19" s="35"/>
       <c r="E19" s="35"/>
     </row>
-    <row r="20" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
     </row>
-    <row r="21" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
     </row>
-    <row r="22" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
     </row>
-    <row r="23" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B23" s="37" t="s">
         <v>13</v>
@@ -2309,9 +2276,9 @@
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
     </row>
-    <row r="24" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="36" t="s">
@@ -2322,9 +2289,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="35"/>
@@ -2333,9 +2300,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B26" s="37" t="s">
         <v>13</v>
@@ -2348,7 +2315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>31</v>
       </c>
@@ -2365,7 +2332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>32</v>
       </c>
@@ -2392,20 +2359,20 @@
   </sheetPr>
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="19" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
@@ -2421,7 +2388,7 @@
       <c r="K1" s="26"/>
       <c r="L1" s="26"/>
     </row>
-    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2437,7 +2404,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
@@ -2453,7 +2420,7 @@
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
@@ -2469,7 +2436,7 @@
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -2485,7 +2452,7 @@
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2501,12 +2468,12 @@
       <c r="K6" s="26"/>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -2519,12 +2486,12 @@
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>18</v>
@@ -2533,22 +2500,22 @@
         <v>19</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H8" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="K8" s="27" t="s">
         <v>8</v>
@@ -2557,9 +2524,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
@@ -2570,12 +2537,12 @@
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
       <c r="J9" s="19" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
     </row>
-    <row r="10" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>26</v>
       </c>
@@ -2588,12 +2555,12 @@
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
     </row>
-    <row r="11" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>27</v>
       </c>
@@ -2606,12 +2573,12 @@
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
       <c r="J11" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
     </row>
-    <row r="12" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>28</v>
       </c>
@@ -2624,12 +2591,12 @@
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
       <c r="J12" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>29</v>
       </c>
@@ -2642,12 +2609,12 @@
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
       <c r="J13" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
     </row>
-    <row r="14" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>30</v>
       </c>
@@ -2660,14 +2627,14 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
       <c r="J14" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -2683,7 +2650,7 @@
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
     </row>
-    <row r="16" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>31</v>
       </c>
@@ -2701,7 +2668,7 @@
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2719,7 +2686,7 @@
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
     </row>
-    <row r="18" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
@@ -2737,47 +2704,47 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
     </row>
-    <row r="19" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>13</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
@@ -2788,14 +2755,14 @@
       <c r="H20" s="19"/>
       <c r="I20" s="24"/>
       <c r="J20" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
     </row>
-    <row r="21" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -2811,9 +2778,9 @@
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
     </row>
-    <row r="22" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
@@ -2824,16 +2791,16 @@
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
       <c r="J22" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K22" s="20"/>
       <c r="L22" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
@@ -2844,14 +2811,14 @@
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
       <c r="J23" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
     </row>
-    <row r="24" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -2862,14 +2829,14 @@
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
       <c r="J24" s="19" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
     </row>
-    <row r="25" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
@@ -2877,19 +2844,19 @@
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="19" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
       <c r="J25" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
     </row>
-    <row r="26" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>13</v>
@@ -2910,14 +2877,14 @@
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
       <c r="J26" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
     </row>
-    <row r="27" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>13</v>
@@ -2938,14 +2905,14 @@
       <c r="H27" s="24"/>
       <c r="I27" s="24"/>
       <c r="J27" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
     </row>
-    <row r="28" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
@@ -2956,88 +2923,88 @@
       <c r="H28" s="24"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
     </row>
-    <row r="29" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="I29" s="19" t="s">
         <v>13</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="L29" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="I30" s="24"/>
       <c r="J30" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="24"/>
@@ -3048,14 +3015,14 @@
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
       <c r="J31" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
     </row>
-    <row r="32" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B32" s="24"/>
       <c r="C32" s="24"/>
@@ -3066,14 +3033,14 @@
       <c r="H32" s="24"/>
       <c r="I32" s="24"/>
       <c r="J32" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
     </row>
-    <row r="33" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -3084,14 +3051,14 @@
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
       <c r="J33" s="19" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
     </row>
-    <row r="34" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
@@ -3102,14 +3069,14 @@
       <c r="H34" s="24"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
     </row>
-    <row r="35" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B35" s="24"/>
       <c r="C35" s="24"/>
@@ -3120,14 +3087,14 @@
       <c r="H35" s="24"/>
       <c r="I35" s="24"/>
       <c r="J35" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
     </row>
-    <row r="36" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
@@ -3138,14 +3105,14 @@
       <c r="H36" s="24"/>
       <c r="I36" s="24"/>
       <c r="J36" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
     </row>
-    <row r="37" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
@@ -3156,14 +3123,14 @@
       <c r="H37" s="24"/>
       <c r="I37" s="24"/>
       <c r="J37" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
     </row>
-    <row r="38" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B38" s="23"/>
       <c r="C38" s="19"/>
@@ -3174,14 +3141,14 @@
       <c r="H38" s="24"/>
       <c r="I38" s="24"/>
       <c r="J38" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
     </row>
-    <row r="39" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
@@ -3192,14 +3159,14 @@
       <c r="H39" s="24"/>
       <c r="I39" s="24"/>
       <c r="J39" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
     </row>
-    <row r="40" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B40" s="23" t="s">
         <v>13</v>
@@ -3224,17 +3191,17 @@
         <v>13</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
     </row>
-    <row r="41" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>13</v>
@@ -3267,9 +3234,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B42" s="29"/>
       <c r="C42" s="24"/>
@@ -3285,7 +3252,7 @@
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
     </row>
-    <row r="43" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>24</v>
       </c>
@@ -3298,12 +3265,12 @@
       <c r="H43" s="24"/>
       <c r="I43" s="19"/>
       <c r="J43" s="19" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
     </row>
-    <row r="44" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>25</v>
       </c>
@@ -3316,14 +3283,14 @@
       <c r="H44" s="24"/>
       <c r="I44" s="24"/>
       <c r="J44" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
     </row>
-    <row r="45" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
@@ -3341,9 +3308,9 @@
       </c>
       <c r="L45" s="20"/>
     </row>
-    <row r="46" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
@@ -3354,16 +3321,16 @@
       <c r="H46" s="24"/>
       <c r="I46" s="19"/>
       <c r="J46" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K46" s="20"/>
       <c r="L46" s="28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
@@ -3374,12 +3341,12 @@
       <c r="H47" s="24"/>
       <c r="I47" s="19"/>
       <c r="J47" s="19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K47" s="20"/>
       <c r="L47" s="20"/>
     </row>
-    <row r="48" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>22</v>
       </c>
@@ -3392,12 +3359,12 @@
       <c r="H48" s="24"/>
       <c r="I48" s="24"/>
       <c r="J48" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K48" s="20"/>
       <c r="L48" s="20"/>
     </row>
-    <row r="49" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>23</v>
       </c>
@@ -3410,14 +3377,14 @@
       <c r="H49" s="24"/>
       <c r="I49" s="24"/>
       <c r="J49" s="19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K49" s="20"/>
       <c r="L49" s="20"/>
     </row>
-    <row r="50" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>13</v>
@@ -3453,9 +3420,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>13</v>
@@ -3491,7 +3458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -3503,7 +3470,7 @@
       <c r="K52" s="21"/>
       <c r="L52" s="21"/>
     </row>
-    <row r="53" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -3515,7 +3482,7 @@
       <c r="K53" s="21"/>
       <c r="L53" s="21"/>
     </row>
-    <row r="54" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -3543,283 +3510,283 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="24"/>
     </row>
-    <row r="11" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="24"/>
     </row>
-    <row r="12" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="24"/>
     </row>
-    <row r="13" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="24"/>
     </row>
-    <row r="14" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="24"/>
     </row>
-    <row r="15" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B15" s="24"/>
     </row>
-    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="24"/>
     </row>
-    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="24"/>
     </row>
-    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="24"/>
     </row>
-    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="23"/>
+    </row>
+    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="23"/>
+    </row>
+    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="23"/>
+    </row>
+    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="23"/>
+    </row>
+    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="23"/>
+    </row>
+    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="23"/>
+    </row>
+    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="23"/>
+    </row>
+    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="23"/>
+    </row>
+    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="23"/>
+    </row>
+    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="23"/>
+    </row>
+    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="23"/>
+    </row>
+    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="23"/>
+    </row>
+    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="23"/>
+    </row>
+    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="23"/>
+    </row>
+    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="23"/>
+    </row>
+    <row r="39" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="23"/>
+    </row>
+    <row r="40" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="23"/>
-    </row>
-    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="23"/>
-    </row>
-    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="23"/>
-    </row>
-    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="23"/>
-    </row>
-    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="23"/>
-    </row>
-    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="23"/>
-    </row>
-    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="23"/>
-    </row>
-    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="23"/>
-    </row>
-    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="23"/>
-    </row>
-    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="23"/>
-    </row>
-    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="23"/>
-    </row>
-    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="23"/>
-    </row>
-    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
+      <c r="B40" s="23"/>
+    </row>
+    <row r="41" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="23"/>
-    </row>
-    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="23"/>
-    </row>
-    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="23"/>
-    </row>
-    <row r="39" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="23"/>
-    </row>
-    <row r="40" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="23"/>
-    </row>
-    <row r="41" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="B41" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B42" s="25"/>
     </row>
-    <row r="43" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>24</v>
       </c>
@@ -3827,43 +3794,43 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B44" s="23"/>
     </row>
-    <row r="45" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B45" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B46" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B47" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="23"/>
     </row>
-    <row r="49" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>23</v>
       </c>
@@ -3879,63 +3846,63 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -3943,19 +3910,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="17"/>
     </row>
-    <row r="10" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="17"/>
     </row>
-    <row r="11" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
@@ -3963,25 +3930,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="17"/>
     </row>
-    <row r="14" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="17"/>
     </row>
-    <row r="15" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -3989,217 +3956,155 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="17"/>
     </row>
-    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="17"/>
     </row>
-    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="17"/>
     </row>
-    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="17"/>
     </row>
-    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="17"/>
     </row>
-    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="17"/>
     </row>
-    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="17"/>
-    </row>
-    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="17"/>
     </row>
-    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="17"/>
     </row>
-    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="17"/>
+    </row>
+    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="17"/>
     </row>
-    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="17"/>
     </row>
-    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="17"/>
     </row>
-    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="17"/>
     </row>
-    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="17"/>
     </row>
-    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="17"/>
-    </row>
-    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="17"/>
     </row>
-    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="17"/>
-    </row>
-    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="17"/>
-    </row>
-    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="17"/>
-    </row>
-    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="17"/>
-    </row>
-    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="17"/>
-    </row>
-    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="17"/>
-    </row>
-    <row r="39" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="17"/>
-    </row>
-    <row r="40" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="17"/>
-    </row>
-    <row r="41" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="17"/>
-    </row>
-    <row r="42" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="17"/>
-    </row>
-    <row r="43" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="17"/>
-    </row>
-    <row r="44" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="17"/>
-    </row>
-    <row r="46" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="19"/>
-      <c r="B46" s="20"/>
-    </row>
-    <row r="47" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="19"/>
-      <c r="B47" s="20"/>
-    </row>
-    <row r="48" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="19"/>
-      <c r="B48" s="20"/>
-    </row>
-    <row r="49" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
-    </row>
-    <row r="50" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="21"/>
-    </row>
-    <row r="51" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="21"/>
-    </row>
-    <row r="52" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B34" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+    </row>
+    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+    </row>
+    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+    </row>
+    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+    </row>
+    <row r="39" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="21"/>
+    </row>
+    <row r="40" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="21"/>
+    </row>
+    <row r="41" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4216,51 +4121,51 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -4268,7 +4173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Updated TOB exclude based on email from Thomas, and ADS release schedules based on Ray Wang tables
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp47837\user\home\zh21490\agage-archive\data\agage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA739285-F331-4B4A-BC2E-AB213CD77ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1343B7-2198-5140-878C-213490A895E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="24300" windowHeight="18280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALE" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="101">
   <si>
     <t># AGAGE LGR data release schedule</t>
   </si>
@@ -327,6 +327,15 @@
   </si>
   <si>
     <t>ADR</t>
+  </si>
+  <si>
+    <t>2004-12-31 00:00</t>
+  </si>
+  <si>
+    <t>2008-04-31 00:00</t>
+  </si>
+  <si>
+    <t>2023-06-01 00:00</t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -531,18 +540,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,6 +556,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -872,54 +890,54 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -939,27 +957,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -980,14 +998,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -995,7 +1013,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1003,7 +1021,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1011,7 +1029,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1019,7 +1037,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1027,7 +1045,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1035,17 +1053,17 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1069,7 +1087,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1077,7 +1095,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1091,7 +1109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1121,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1133,58 +1151,58 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1195,19 +1213,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1231,58 +1249,58 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1293,7 +1311,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1302,7 +1320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1311,7 +1329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1319,7 +1337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1327,7 +1345,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1354,57 +1372,57 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1412,7 +1430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1420,7 +1438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -1444,57 +1462,57 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1502,13 +1520,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -1530,60 +1548,60 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="40"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="36"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="36"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="36"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="36"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="40"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="36"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="40"/>
-    </row>
-    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36"/>
+    </row>
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1603,47 +1621,47 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="40"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="40"/>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="36"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="40"/>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="36"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="40"/>
-    </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="36"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="40"/>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="36"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="40"/>
-    </row>
-    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="36"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="41"/>
+      <c r="B15" s="37"/>
       <c r="D15" t="s">
         <v>13</v>
       </c>
@@ -1664,17 +1682,17 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1683,7 +1701,7 @@
       <c r="E1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1692,7 +1710,7 @@
       <c r="E2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1701,7 +1719,7 @@
       <c r="E3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1710,7 +1728,7 @@
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1719,7 +1737,7 @@
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1728,11 +1746,11 @@
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
       <c r="C7" s="1"/>
@@ -1740,7 +1758,7 @@
       <c r="E7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1763,7 +1781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
@@ -1776,7 +1794,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>55</v>
       </c>
@@ -1789,7 +1807,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>84</v>
       </c>
@@ -1812,7 +1830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
@@ -1835,7 +1853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1848,7 +1866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -1859,7 +1877,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -1882,7 +1900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>43</v>
       </c>
@@ -1895,7 +1913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
@@ -1916,7 +1934,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
@@ -1946,53 +1964,53 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2001,7 +2019,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -2012,7 +2030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -2032,20 +2050,20 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2054,7 +2072,7 @@
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2063,7 +2081,7 @@
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2072,7 +2090,7 @@
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2081,7 +2099,7 @@
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2090,7 +2108,7 @@
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2099,18 +2117,18 @@
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -2127,223 +2145,343 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-    </row>
-    <row r="10" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-    </row>
-    <row r="11" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-    </row>
-    <row r="12" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-    </row>
-    <row r="13" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="35"/>
-    </row>
-    <row r="14" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-    </row>
-    <row r="15" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="35"/>
-    </row>
-    <row r="16" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="36" t="s">
+      <c r="B16" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="36" t="s">
+      <c r="D16" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-    </row>
-    <row r="18" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-    </row>
-    <row r="19" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-    </row>
-    <row r="20" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-    </row>
-    <row r="21" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-    </row>
-    <row r="22" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-    </row>
-    <row r="23" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-    </row>
-    <row r="24" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="36" t="s">
+      <c r="B28" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="41" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2363,16 +2501,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="19" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
@@ -2388,7 +2526,7 @@
       <c r="K1" s="26"/>
       <c r="L1" s="26"/>
     </row>
-    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2404,7 +2542,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
@@ -2420,7 +2558,7 @@
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
@@ -2436,7 +2574,7 @@
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -2452,7 +2590,7 @@
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2468,11 +2606,11 @@
       <c r="K6" s="26"/>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
       <c r="C7" s="16"/>
@@ -2486,7 +2624,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -2524,7 +2662,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>49</v>
       </c>
@@ -2542,7 +2680,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
     </row>
-    <row r="10" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>26</v>
       </c>
@@ -2560,7 +2698,7 @@
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
     </row>
-    <row r="11" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>27</v>
       </c>
@@ -2578,7 +2716,7 @@
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
     </row>
-    <row r="12" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>28</v>
       </c>
@@ -2596,7 +2734,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>29</v>
       </c>
@@ -2614,7 +2752,7 @@
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
     </row>
-    <row r="14" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>30</v>
       </c>
@@ -2632,7 +2770,7 @@
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>50</v>
       </c>
@@ -2650,7 +2788,7 @@
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
     </row>
-    <row r="16" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>31</v>
       </c>
@@ -2668,7 +2806,7 @@
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2686,7 +2824,7 @@
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
     </row>
-    <row r="18" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
@@ -2704,7 +2842,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
     </row>
-    <row r="19" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>51</v>
       </c>
@@ -2742,7 +2880,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>34</v>
       </c>
@@ -2760,7 +2898,7 @@
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
     </row>
-    <row r="21" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>52</v>
       </c>
@@ -2778,7 +2916,7 @@
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
     </row>
-    <row r="22" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>35</v>
       </c>
@@ -2798,7 +2936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>37</v>
       </c>
@@ -2816,7 +2954,7 @@
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
     </row>
-    <row r="24" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>53</v>
       </c>
@@ -2834,7 +2972,7 @@
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
     </row>
-    <row r="25" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>36</v>
       </c>
@@ -2854,7 +2992,7 @@
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
     </row>
-    <row r="26" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>54</v>
       </c>
@@ -2882,7 +3020,7 @@
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
     </row>
-    <row r="27" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>55</v>
       </c>
@@ -2910,7 +3048,7 @@
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
     </row>
-    <row r="28" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>56</v>
       </c>
@@ -2928,7 +3066,7 @@
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
     </row>
-    <row r="29" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>57</v>
       </c>
@@ -2966,7 +3104,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>58</v>
       </c>
@@ -3002,7 +3140,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>38</v>
       </c>
@@ -3020,7 +3158,7 @@
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
     </row>
-    <row r="32" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>39</v>
       </c>
@@ -3038,7 +3176,7 @@
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
     </row>
-    <row r="33" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>59</v>
       </c>
@@ -3056,7 +3194,7 @@
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
     </row>
-    <row r="34" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>60</v>
       </c>
@@ -3074,7 +3212,7 @@
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
     </row>
-    <row r="35" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>40</v>
       </c>
@@ -3092,7 +3230,7 @@
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
     </row>
-    <row r="36" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>41</v>
       </c>
@@ -3110,7 +3248,7 @@
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
     </row>
-    <row r="37" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>42</v>
       </c>
@@ -3128,7 +3266,7 @@
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
     </row>
-    <row r="38" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
         <v>43</v>
       </c>
@@ -3146,7 +3284,7 @@
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
     </row>
-    <row r="39" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>61</v>
       </c>
@@ -3164,7 +3302,7 @@
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
     </row>
-    <row r="40" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>62</v>
       </c>
@@ -3196,7 +3334,7 @@
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
     </row>
-    <row r="41" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>44</v>
       </c>
@@ -3234,7 +3372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>45</v>
       </c>
@@ -3252,7 +3390,7 @@
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
     </row>
-    <row r="43" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>24</v>
       </c>
@@ -3270,7 +3408,7 @@
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
     </row>
-    <row r="44" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>25</v>
       </c>
@@ -3288,7 +3426,7 @@
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
     </row>
-    <row r="45" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>63</v>
       </c>
@@ -3308,7 +3446,7 @@
       </c>
       <c r="L45" s="20"/>
     </row>
-    <row r="46" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>64</v>
       </c>
@@ -3328,7 +3466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>65</v>
       </c>
@@ -3346,7 +3484,7 @@
       <c r="K47" s="20"/>
       <c r="L47" s="20"/>
     </row>
-    <row r="48" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>22</v>
       </c>
@@ -3364,7 +3502,7 @@
       <c r="K48" s="20"/>
       <c r="L48" s="20"/>
     </row>
-    <row r="49" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
         <v>23</v>
       </c>
@@ -3382,7 +3520,7 @@
       <c r="K49" s="20"/>
       <c r="L49" s="20"/>
     </row>
-    <row r="50" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>47</v>
       </c>
@@ -3420,7 +3558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>46</v>
       </c>
@@ -3458,7 +3596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -3470,7 +3608,7 @@
       <c r="K52" s="21"/>
       <c r="L52" s="21"/>
     </row>
-    <row r="53" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -3482,7 +3620,7 @@
       <c r="K53" s="21"/>
       <c r="L53" s="21"/>
     </row>
-    <row r="54" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -3506,335 +3644,337 @@
   </sheetPr>
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="42"/>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="42"/>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="42"/>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="42"/>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="42"/>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42"/>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="24"/>
-    </row>
-    <row r="11" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+    </row>
+    <row r="11" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="24"/>
-    </row>
-    <row r="12" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="44"/>
+    </row>
+    <row r="12" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="24"/>
-    </row>
-    <row r="13" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+    </row>
+    <row r="13" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="24"/>
-    </row>
-    <row r="14" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="44"/>
+    </row>
+    <row r="14" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="24"/>
-    </row>
-    <row r="15" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="44"/>
+    </row>
+    <row r="15" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="24"/>
-    </row>
-    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="44"/>
+    </row>
+    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="24"/>
-    </row>
-    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="44"/>
+    </row>
+    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="24"/>
-    </row>
-    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="44"/>
+    </row>
+    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="24"/>
-    </row>
-    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="44"/>
+    </row>
+    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="23"/>
-    </row>
-    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="44"/>
+    </row>
+    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="23"/>
-    </row>
-    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="44"/>
+    </row>
+    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="23"/>
-    </row>
-    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="44"/>
+    </row>
+    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="23"/>
-    </row>
-    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="44"/>
+    </row>
+    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="23"/>
-    </row>
-    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="44"/>
+    </row>
+    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="23"/>
-    </row>
-    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="44"/>
+    </row>
+    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="23"/>
-    </row>
-    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="44"/>
+    </row>
+    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="23"/>
-    </row>
-    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="23"/>
-    </row>
-    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="44"/>
+    </row>
+    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="23"/>
-    </row>
-    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="44"/>
+    </row>
+    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="23"/>
-    </row>
-    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="44"/>
+    </row>
+    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="23"/>
-    </row>
-    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="44"/>
+    </row>
+    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="23"/>
-    </row>
-    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="44"/>
+    </row>
+    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="23"/>
-    </row>
-    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="44"/>
+    </row>
+    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="23"/>
-    </row>
-    <row r="39" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="44"/>
+    </row>
+    <row r="39" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="23"/>
-    </row>
-    <row r="40" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="44"/>
+    </row>
+    <row r="40" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="23"/>
-    </row>
-    <row r="41" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="44"/>
+    </row>
+    <row r="41" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="25"/>
-    </row>
-    <row r="43" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="45"/>
+    </row>
+    <row r="43" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="23"/>
-    </row>
-    <row r="45" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="44"/>
+    </row>
+    <row r="45" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="23"/>
-    </row>
-    <row r="49" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="44"/>
+    </row>
+    <row r="49" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="23"/>
+      <c r="B49" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3848,61 +3988,61 @@
   </sheetPr>
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -3910,19 +4050,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="17"/>
     </row>
-    <row r="10" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="17"/>
     </row>
-    <row r="11" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
@@ -3930,25 +4070,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="17"/>
     </row>
-    <row r="14" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="17"/>
     </row>
-    <row r="15" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -3956,43 +4096,43 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="17"/>
     </row>
-    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="17"/>
     </row>
-    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="17"/>
     </row>
-    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="17"/>
     </row>
-    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="17"/>
     </row>
-    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="17"/>
     </row>
-    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>35</v>
       </c>
@@ -4000,55 +4140,55 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="17"/>
     </row>
-    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="17"/>
     </row>
-    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="17"/>
     </row>
-    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="17"/>
     </row>
-    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="17"/>
     </row>
-    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="17"/>
     </row>
-    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="17"/>
     </row>
-    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="17"/>
     </row>
-    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>44</v>
       </c>
@@ -4056,13 +4196,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="17"/>
     </row>
-    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>46</v>
       </c>
@@ -4070,7 +4210,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>47</v>
       </c>
@@ -4078,33 +4218,33 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
     </row>
-    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="20"/>
     </row>
-    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
       <c r="B37" s="20"/>
     </row>
-    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
       <c r="B38" s="20"/>
     </row>
-    <row r="39" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="21"/>
     </row>
-    <row r="40" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="21"/>
     </row>
-    <row r="41" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4121,51 +4261,51 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -4173,7 +4313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
April has 30 days, idiot
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/dagage2_home/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1343B7-2198-5140-878C-213490A895E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9807ACEF-1872-9740-84C9-21A04CF56124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="24300" windowHeight="18280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,10 +332,10 @@
     <t>2004-12-31 00:00</t>
   </si>
   <si>
-    <t>2008-04-31 00:00</t>
-  </si>
-  <si>
     <t>2023-06-01 00:00</t>
+  </si>
+  <si>
+    <t>2008-04-30 00:00</t>
   </si>
 </sst>
 </file>
@@ -2051,7 +2051,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2156,7 +2156,7 @@
         <v>98</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E9" s="41" t="s">
         <v>92</v>
@@ -2173,7 +2173,7 @@
         <v>98</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E10" s="41" t="s">
         <v>92</v>
@@ -2190,7 +2190,7 @@
         <v>98</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E11" s="41" t="s">
         <v>92</v>
@@ -2207,7 +2207,7 @@
         <v>98</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E12" s="41" t="s">
         <v>92</v>
@@ -2241,7 +2241,7 @@
         <v>98</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E14" s="41" t="s">
         <v>92</v>
@@ -2292,7 +2292,7 @@
         <v>98</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E17" s="41" t="s">
         <v>92</v>
@@ -2309,7 +2309,7 @@
         <v>98</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E18" s="41" t="s">
         <v>92</v>
@@ -2326,7 +2326,7 @@
         <v>98</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E19" s="41" t="s">
         <v>92</v>
@@ -2343,7 +2343,7 @@
         <v>98</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="41" t="s">
         <v>92</v>
@@ -2360,7 +2360,7 @@
         <v>98</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E21" s="41" t="s">
         <v>92</v>
@@ -2377,7 +2377,7 @@
         <v>98</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E22" s="41" t="s">
         <v>92</v>
@@ -2394,7 +2394,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>92</v>
@@ -2411,7 +2411,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E24" s="41" t="s">
         <v>13</v>
@@ -2428,7 +2428,7 @@
         <v>98</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25" s="41" t="s">
         <v>13</v>
@@ -2445,7 +2445,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E26" s="41" t="s">
         <v>13</v>
@@ -2479,7 +2479,7 @@
         <v>13</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E28" s="41" t="s">
         <v>13</v>
@@ -3695,7 +3695,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Remove withold on MHD CO data
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/dagage2_home/code/agage-archive/data/agage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp09676\user\home\zh21490\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9807ACEF-1872-9740-84C9-21A04CF56124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF5EF2C-8971-4650-8B86-64C8255E1897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="24300" windowHeight="18280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALE" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="101">
   <si>
     <t># AGAGE LGR data release schedule</t>
   </si>
@@ -890,46 +890,46 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -937,7 +937,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -957,27 +957,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -998,14 +998,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1029,7 +1029,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1053,7 +1053,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1063,7 +1063,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1095,7 +1095,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1151,50 +1151,50 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1213,19 +1213,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1249,50 +1249,50 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1372,49 +1372,49 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -1462,49 +1462,49 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1520,13 +1520,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -1548,52 +1548,52 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="36"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="36"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="36"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="36"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="36"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="36"/>
     </row>
-    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1621,43 +1621,43 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="36"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="36"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="36"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="36"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="36"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="36"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1678,21 +1678,21 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1701,7 +1701,7 @@
       <c r="E1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1710,7 +1710,7 @@
       <c r="E2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="E3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1737,7 +1737,7 @@
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1758,7 +1758,7 @@
       <c r="E7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>55</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>84</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>43</v>
       </c>
@@ -1913,13 +1913,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1934,7 +1932,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
@@ -1967,50 +1965,50 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2019,7 +2017,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -2030,7 +2028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -2050,20 +2048,20 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" style="35" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2072,7 +2070,7 @@
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2081,7 +2079,7 @@
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2090,7 +2088,7 @@
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2099,7 +2097,7 @@
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2108,7 +2106,7 @@
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2117,7 +2115,7 @@
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2128,7 +2126,7 @@
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -2145,7 +2143,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
@@ -2162,7 +2160,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>28</v>
       </c>
@@ -2179,7 +2177,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>30</v>
       </c>
@@ -2196,7 +2194,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>33</v>
       </c>
@@ -2213,7 +2211,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>34</v>
       </c>
@@ -2230,7 +2228,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>53</v>
       </c>
@@ -2247,7 +2245,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>36</v>
       </c>
@@ -2264,7 +2262,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>52</v>
       </c>
@@ -2281,7 +2279,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>39</v>
       </c>
@@ -2298,7 +2296,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>59</v>
       </c>
@@ -2315,7 +2313,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>40</v>
       </c>
@@ -2332,7 +2330,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>41</v>
       </c>
@@ -2349,7 +2347,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>42</v>
       </c>
@@ -2366,7 +2364,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>43</v>
       </c>
@@ -2383,7 +2381,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>61</v>
       </c>
@@ -2400,7 +2398,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>44</v>
       </c>
@@ -2417,7 +2415,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>45</v>
       </c>
@@ -2434,7 +2432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>50</v>
       </c>
@@ -2451,7 +2449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>31</v>
       </c>
@@ -2468,7 +2466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>32</v>
       </c>
@@ -2501,16 +2499,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="19" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
@@ -2526,7 +2524,7 @@
       <c r="K1" s="26"/>
       <c r="L1" s="26"/>
     </row>
-    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2542,7 +2540,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
@@ -2558,7 +2556,7 @@
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
@@ -2574,7 +2572,7 @@
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -2590,7 +2588,7 @@
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2606,7 +2604,7 @@
       <c r="K6" s="26"/>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2624,7 +2622,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -2662,7 +2660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>49</v>
       </c>
@@ -2680,7 +2678,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
     </row>
-    <row r="10" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>26</v>
       </c>
@@ -2698,7 +2696,7 @@
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
     </row>
-    <row r="11" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>27</v>
       </c>
@@ -2716,7 +2714,7 @@
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
     </row>
-    <row r="12" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>28</v>
       </c>
@@ -2734,7 +2732,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>29</v>
       </c>
@@ -2752,7 +2750,7 @@
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
     </row>
-    <row r="14" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>30</v>
       </c>
@@ -2770,7 +2768,7 @@
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>50</v>
       </c>
@@ -2788,7 +2786,7 @@
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
     </row>
-    <row r="16" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>31</v>
       </c>
@@ -2806,7 +2804,7 @@
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2824,7 +2822,7 @@
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
     </row>
-    <row r="18" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
@@ -2842,7 +2840,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
     </row>
-    <row r="19" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>51</v>
       </c>
@@ -2880,7 +2878,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>34</v>
       </c>
@@ -2898,7 +2896,7 @@
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
     </row>
-    <row r="21" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>52</v>
       </c>
@@ -2916,7 +2914,7 @@
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
     </row>
-    <row r="22" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>35</v>
       </c>
@@ -2936,7 +2934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>37</v>
       </c>
@@ -2954,7 +2952,7 @@
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
     </row>
-    <row r="24" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>53</v>
       </c>
@@ -2972,7 +2970,7 @@
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
     </row>
-    <row r="25" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>36</v>
       </c>
@@ -2992,7 +2990,7 @@
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
     </row>
-    <row r="26" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>54</v>
       </c>
@@ -3020,7 +3018,7 @@
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
     </row>
-    <row r="27" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>55</v>
       </c>
@@ -3048,7 +3046,7 @@
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
     </row>
-    <row r="28" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>56</v>
       </c>
@@ -3066,7 +3064,7 @@
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
     </row>
-    <row r="29" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>57</v>
       </c>
@@ -3104,7 +3102,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>58</v>
       </c>
@@ -3140,7 +3138,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>38</v>
       </c>
@@ -3158,7 +3156,7 @@
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
     </row>
-    <row r="32" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>39</v>
       </c>
@@ -3176,7 +3174,7 @@
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
     </row>
-    <row r="33" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>59</v>
       </c>
@@ -3194,7 +3192,7 @@
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
     </row>
-    <row r="34" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>60</v>
       </c>
@@ -3212,7 +3210,7 @@
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
     </row>
-    <row r="35" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>40</v>
       </c>
@@ -3230,7 +3228,7 @@
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
     </row>
-    <row r="36" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>41</v>
       </c>
@@ -3248,7 +3246,7 @@
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
     </row>
-    <row r="37" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>42</v>
       </c>
@@ -3266,7 +3264,7 @@
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
     </row>
-    <row r="38" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>43</v>
       </c>
@@ -3284,7 +3282,7 @@
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
     </row>
-    <row r="39" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>61</v>
       </c>
@@ -3302,7 +3300,7 @@
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
     </row>
-    <row r="40" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>62</v>
       </c>
@@ -3334,7 +3332,7 @@
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
     </row>
-    <row r="41" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>44</v>
       </c>
@@ -3372,7 +3370,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>45</v>
       </c>
@@ -3390,7 +3388,7 @@
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
     </row>
-    <row r="43" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>24</v>
       </c>
@@ -3408,7 +3406,7 @@
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
     </row>
-    <row r="44" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>25</v>
       </c>
@@ -3426,7 +3424,7 @@
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
     </row>
-    <row r="45" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>63</v>
       </c>
@@ -3446,7 +3444,7 @@
       </c>
       <c r="L45" s="20"/>
     </row>
-    <row r="46" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>64</v>
       </c>
@@ -3466,7 +3464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>65</v>
       </c>
@@ -3484,7 +3482,7 @@
       <c r="K47" s="20"/>
       <c r="L47" s="20"/>
     </row>
-    <row r="48" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>22</v>
       </c>
@@ -3502,7 +3500,7 @@
       <c r="K48" s="20"/>
       <c r="L48" s="20"/>
     </row>
-    <row r="49" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>23</v>
       </c>
@@ -3520,7 +3518,7 @@
       <c r="K49" s="20"/>
       <c r="L49" s="20"/>
     </row>
-    <row r="50" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>47</v>
       </c>
@@ -3558,7 +3556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>46</v>
       </c>
@@ -3596,7 +3594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -3608,7 +3606,7 @@
       <c r="K52" s="21"/>
       <c r="L52" s="21"/>
     </row>
-    <row r="53" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -3620,7 +3618,7 @@
       <c r="K53" s="21"/>
       <c r="L53" s="21"/>
     </row>
-    <row r="54" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -3648,49 +3646,49 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="42"/>
     </row>
-    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="42"/>
     </row>
-    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="42"/>
     </row>
-    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="42"/>
     </row>
-    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="42"/>
     </row>
-    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="42"/>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3698,7 +3696,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -3706,7 +3704,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>49</v>
       </c>
@@ -3714,61 +3712,61 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="44"/>
     </row>
-    <row r="11" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="44"/>
     </row>
-    <row r="12" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="44"/>
     </row>
-    <row r="13" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="44"/>
     </row>
-    <row r="14" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="44"/>
     </row>
-    <row r="15" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="44"/>
     </row>
-    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="44"/>
     </row>
-    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="44"/>
     </row>
-    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="44"/>
     </row>
-    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>51</v>
       </c>
@@ -3776,13 +3774,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="44"/>
     </row>
-    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>52</v>
       </c>
@@ -3790,43 +3788,43 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="44"/>
     </row>
-    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="44"/>
     </row>
-    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="44"/>
     </row>
-    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="44"/>
     </row>
-    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="44"/>
     </row>
-    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B27" s="44"/>
     </row>
-    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>56</v>
       </c>
@@ -3834,7 +3832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>57</v>
       </c>
@@ -3842,7 +3840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>58</v>
       </c>
@@ -3850,25 +3848,25 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="44"/>
     </row>
-    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="44"/>
     </row>
-    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>59</v>
       </c>
       <c r="B33" s="44"/>
     </row>
-    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>60</v>
       </c>
@@ -3876,43 +3874,43 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="44"/>
     </row>
-    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="44"/>
     </row>
-    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="44"/>
     </row>
-    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="44"/>
     </row>
-    <row r="39" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>61</v>
       </c>
       <c r="B39" s="44"/>
     </row>
-    <row r="40" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>62</v>
       </c>
       <c r="B40" s="44"/>
     </row>
-    <row r="41" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>44</v>
       </c>
@@ -3920,13 +3918,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="45"/>
     </row>
-    <row r="43" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>24</v>
       </c>
@@ -3934,13 +3932,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B44" s="44"/>
     </row>
-    <row r="45" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>63</v>
       </c>
@@ -3948,7 +3946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>64</v>
       </c>
@@ -3956,7 +3954,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>65</v>
       </c>
@@ -3964,13 +3962,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="44"/>
     </row>
-    <row r="49" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>23</v>
       </c>
@@ -3992,49 +3990,49 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4042,7 +4040,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -4050,19 +4048,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="17"/>
     </row>
-    <row r="10" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="17"/>
     </row>
-    <row r="11" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
@@ -4070,25 +4068,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="17"/>
     </row>
-    <row r="14" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="17"/>
     </row>
-    <row r="15" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -4096,43 +4094,43 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="17"/>
     </row>
-    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="17"/>
     </row>
-    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="17"/>
     </row>
-    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="17"/>
     </row>
-    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="17"/>
     </row>
-    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="17"/>
     </row>
-    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>35</v>
       </c>
@@ -4140,55 +4138,55 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="17"/>
     </row>
-    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="17"/>
     </row>
-    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="17"/>
     </row>
-    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="17"/>
     </row>
-    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="17"/>
     </row>
-    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="17"/>
     </row>
-    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="17"/>
     </row>
-    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="17"/>
     </row>
-    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>44</v>
       </c>
@@ -4196,13 +4194,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="17"/>
     </row>
-    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>46</v>
       </c>
@@ -4210,7 +4208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>47</v>
       </c>
@@ -4218,33 +4216,33 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
     </row>
-    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" s="20"/>
     </row>
-    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="20"/>
     </row>
-    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="20"/>
     </row>
-    <row r="39" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="21"/>
     </row>
-    <row r="40" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="21"/>
     </row>
-    <row r="41" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4261,43 +4259,43 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4305,7 +4303,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -4313,7 +4311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
release: change date format to text format
</commit_message>
<xml_diff>
--- a/data/agage/data_release_schedule.xlsx
+++ b/data/agage/data_release_schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp24683\user\home\zh21490\agage-archive\data\agage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp51539\home\zh21490\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EB2018-E129-4D40-AF12-004E00BDDBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812BDCDC-1619-4833-AC51-94F9B95B9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALE" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="105">
   <si>
     <t># AGAGE LGR data release schedule</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>2008-08-15 00:00</t>
+  </si>
+  <si>
+    <t>2005-01-12 00:00</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -567,15 +570,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,6 +587,12 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1552,7 +1552,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="43" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -1562,37 +1562,37 @@
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="41"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="41"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="44"/>
+      <c r="B4" s="41"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="44"/>
+      <c r="B5" s="41"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="44"/>
+      <c r="B6" s="41"/>
     </row>
     <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1626,43 +1626,43 @@
       <c r="A9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="44"/>
+      <c r="B9" s="41"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="44"/>
+      <c r="B10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="44"/>
+      <c r="B11" s="41"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="44"/>
+      <c r="B12" s="41"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="44"/>
+      <c r="B13" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="44"/>
+      <c r="B14" s="41"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="45"/>
+      <c r="B15" s="42"/>
       <c r="D15" t="s">
         <v>14</v>
       </c>
@@ -1882,7 +1882,7 @@
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="43"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
         <v>97</v>
@@ -2061,16 +2061,16 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2159,16 +2159,16 @@
       <c r="A9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2176,16 +2176,16 @@
       <c r="A10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2193,16 +2193,16 @@
       <c r="A11" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2210,16 +2210,16 @@
       <c r="A12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="38">
-        <v>38364</v>
-      </c>
-      <c r="C12" s="39" t="s">
+      <c r="B12" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2227,16 +2227,16 @@
       <c r="A13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="40" t="s">
+      <c r="D13" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2244,16 +2244,16 @@
       <c r="A14" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2261,16 +2261,16 @@
       <c r="A15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="40" t="s">
+      <c r="D15" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2278,16 +2278,16 @@
       <c r="A16" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="40" t="s">
+      <c r="D16" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="45" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2295,16 +2295,16 @@
       <c r="A17" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2312,16 +2312,16 @@
       <c r="A18" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2329,16 +2329,16 @@
       <c r="A19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2346,16 +2346,16 @@
       <c r="A20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2363,16 +2363,16 @@
       <c r="A21" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2380,16 +2380,16 @@
       <c r="A22" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2397,16 +2397,16 @@
       <c r="A23" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="40" t="s">
+      <c r="B23" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="45" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2414,16 +2414,16 @@
       <c r="A24" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="40" t="s">
+      <c r="C24" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="45" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2431,16 +2431,16 @@
       <c r="A25" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E25" s="45" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2448,16 +2448,16 @@
       <c r="A26" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="40" t="s">
+      <c r="B26" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="45" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2465,16 +2465,16 @@
       <c r="A27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="40" t="s">
+      <c r="B27" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="45" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2482,16 +2482,16 @@
       <c r="A28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="40" t="s">
+      <c r="B28" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="45" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2507,7 +2507,9 @@
   </sheetPr>
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>